<commit_message>
updated doc of score compuation and features
</commit_message>
<xml_diff>
--- a/Doc/AutomaticScoreComputationStrategies.xlsx
+++ b/Doc/AutomaticScoreComputationStrategies.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bockisch/Research Drive/IO4 Validation/UMR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bockisch/git/QPED-O4/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4239F6A0-6DCF-2841-961E-0C61A3280D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B058FDE-7A17-184E-99A1-540D980835F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="900" windowWidth="30480" windowHeight="18320" xr2:uid="{39EE1716-99E5-DB4E-B57C-F12671B410C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19180" xr2:uid="{39EE1716-99E5-DB4E-B57C-F12671B410C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +32,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>% positive examples selected</t>
   </si>
   <si>
     <t>% negative examples</t>
+  </si>
+  <si>
+    <t>&lt;--- Current implementation</t>
   </si>
 </sst>
 </file>
@@ -76,10 +79,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B22464D-0FB5-974A-8DE3-C05B1028247C}">
-  <dimension ref="A1:W48"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="Z51" sqref="Z51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +431,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
@@ -520,7 +523,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="1"/>
       <c r="B2">
         <f>B1-0.05</f>
         <v>0.95</v>
@@ -611,7 +614,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="1"/>
       <c r="B3">
         <f t="shared" ref="B3:B20" si="2">B2-0.05</f>
         <v>0.89999999999999991</v>
@@ -702,7 +705,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
       <c r="B4">
         <f t="shared" si="2"/>
         <v>0.84999999999999987</v>
@@ -793,7 +796,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
       <c r="B5">
         <f t="shared" si="2"/>
         <v>0.79999999999999982</v>
@@ -884,7 +887,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
       <c r="B6">
         <f t="shared" si="2"/>
         <v>0.74999999999999978</v>
@@ -975,7 +978,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7">
         <f t="shared" si="2"/>
         <v>0.69999999999999973</v>
@@ -1066,7 +1069,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
       <c r="B8">
         <f t="shared" si="2"/>
         <v>0.64999999999999969</v>
@@ -1157,7 +1160,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9">
         <f t="shared" si="2"/>
         <v>0.59999999999999964</v>
@@ -1248,7 +1251,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
       <c r="B10">
         <f t="shared" si="2"/>
         <v>0.5499999999999996</v>
@@ -1339,7 +1342,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11">
         <f t="shared" si="2"/>
         <v>0.49999999999999961</v>
@@ -1430,7 +1433,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="1"/>
       <c r="B12">
         <f t="shared" si="2"/>
         <v>0.44999999999999962</v>
@@ -1521,7 +1524,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
       <c r="B13">
         <f t="shared" si="2"/>
         <v>0.39999999999999963</v>
@@ -1612,7 +1615,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="1"/>
       <c r="B14">
         <f t="shared" si="2"/>
         <v>0.34999999999999964</v>
@@ -1703,7 +1706,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="1"/>
       <c r="B15">
         <f t="shared" si="2"/>
         <v>0.29999999999999966</v>
@@ -1794,7 +1797,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="1"/>
       <c r="B16">
         <f t="shared" si="2"/>
         <v>0.24999999999999967</v>
@@ -1885,7 +1888,7 @@
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="1"/>
       <c r="B17">
         <f t="shared" si="2"/>
         <v>0.19999999999999968</v>
@@ -1976,7 +1979,7 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="1"/>
       <c r="B18">
         <f t="shared" si="2"/>
         <v>0.14999999999999969</v>
@@ -2067,7 +2070,7 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="B19">
         <f t="shared" si="2"/>
         <v>9.9999999999999686E-2</v>
@@ -2158,7 +2161,7 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
       <c r="B20">
         <f t="shared" si="2"/>
         <v>4.9999999999999684E-2</v>
@@ -2249,7 +2252,7 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="1"/>
       <c r="B21">
         <v>0</v>
       </c>
@@ -2424,32 +2427,32 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B26">
@@ -2541,7 +2544,7 @@
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="1"/>
       <c r="B27">
         <f>B26-0.05</f>
         <v>0.95</v>
@@ -2632,7 +2635,7 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="1"/>
       <c r="B28">
         <f t="shared" ref="B28:B45" si="9">B27-0.05</f>
         <v>0.89999999999999991</v>
@@ -2723,7 +2726,7 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="1"/>
       <c r="B29">
         <f t="shared" si="9"/>
         <v>0.84999999999999987</v>
@@ -2814,7 +2817,7 @@
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="1"/>
       <c r="B30">
         <f t="shared" si="9"/>
         <v>0.79999999999999982</v>
@@ -2905,7 +2908,7 @@
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
       <c r="B31">
         <f t="shared" si="9"/>
         <v>0.74999999999999978</v>
@@ -2996,7 +2999,7 @@
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1"/>
       <c r="B32">
         <f t="shared" si="9"/>
         <v>0.69999999999999973</v>
@@ -3087,7 +3090,7 @@
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1"/>
       <c r="B33">
         <f t="shared" si="9"/>
         <v>0.64999999999999969</v>
@@ -3178,7 +3181,7 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="1"/>
       <c r="B34">
         <f t="shared" si="9"/>
         <v>0.59999999999999964</v>
@@ -3269,7 +3272,7 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="1"/>
       <c r="B35">
         <f t="shared" si="9"/>
         <v>0.5499999999999996</v>
@@ -3360,7 +3363,7 @@
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+      <c r="A36" s="1"/>
       <c r="B36">
         <f t="shared" si="9"/>
         <v>0.49999999999999961</v>
@@ -3451,7 +3454,7 @@
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
+      <c r="A37" s="1"/>
       <c r="B37">
         <f t="shared" si="9"/>
         <v>0.44999999999999962</v>
@@ -3542,7 +3545,7 @@
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
+      <c r="A38" s="1"/>
       <c r="B38">
         <f t="shared" si="9"/>
         <v>0.39999999999999963</v>
@@ -3633,7 +3636,7 @@
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
+      <c r="A39" s="1"/>
       <c r="B39">
         <f t="shared" si="9"/>
         <v>0.34999999999999964</v>
@@ -3724,7 +3727,7 @@
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
+      <c r="A40" s="1"/>
       <c r="B40">
         <f t="shared" si="9"/>
         <v>0.29999999999999966</v>
@@ -3815,7 +3818,7 @@
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A41" s="1"/>
       <c r="B41">
         <f t="shared" si="9"/>
         <v>0.24999999999999967</v>
@@ -3906,7 +3909,7 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" s="1"/>
       <c r="B42">
         <f t="shared" si="9"/>
         <v>0.19999999999999968</v>
@@ -3997,7 +4000,7 @@
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
+      <c r="A43" s="1"/>
       <c r="B43">
         <f t="shared" si="9"/>
         <v>0.14999999999999969</v>
@@ -4088,7 +4091,7 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
+      <c r="A44" s="1"/>
       <c r="B44">
         <f t="shared" si="9"/>
         <v>9.9999999999999686E-2</v>
@@ -4179,7 +4182,7 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
+      <c r="A45" s="1"/>
       <c r="B45">
         <f t="shared" si="9"/>
         <v>4.9999999999999684E-2</v>
@@ -4270,7 +4273,7 @@
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
+      <c r="A46" s="1"/>
       <c r="B46">
         <v>0</v>
       </c>
@@ -4445,38 +4448,2112 @@
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-      <c r="W48" s="1"/>
+      <c r="C48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <f>ROUND((($B52-C$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:W51" si="13">ROUND((($B52-D$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52">
+        <f>B51-0.05</f>
+        <v>0.95</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:C71" si="14">ROUND((($B53-C$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ref="D52:D71" si="15">ROUND((($B53-D$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <f t="shared" ref="E52:E71" si="16">ROUND((($B53-E$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <f t="shared" ref="F52:F71" si="17">ROUND((($B53-F$22) + 1) * 2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52:G71" si="18">ROUND((($B53-G$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <f t="shared" ref="H52:H71" si="19">ROUND((($B53-H$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52:I71" si="20">ROUND((($B53-I$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <f t="shared" ref="J52:J71" si="21">ROUND((($B53-J$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="K52">
+        <f t="shared" ref="K52:K71" si="22">ROUND((($B53-K$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <f t="shared" ref="L52:L71" si="23">ROUND((($B53-L$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52:M71" si="24">ROUND((($B53-M$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52:N71" si="25">ROUND((($B53-N$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="O52">
+        <f t="shared" ref="O52:O71" si="26">ROUND((($B53-O$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="P52">
+        <f t="shared" ref="P52:P71" si="27">ROUND((($B53-P$22) + 1) * 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" ref="Q52:Q71" si="28">ROUND((($B53-Q$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="R52">
+        <f t="shared" ref="R52:R71" si="29">ROUND((($B53-R$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="S52">
+        <f t="shared" ref="S52:S71" si="30">ROUND((($B53-S$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="T52">
+        <f t="shared" ref="T52:T71" si="31">ROUND((($B53-T$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="U52">
+        <f t="shared" ref="U52:U71" si="32">ROUND((($B53-U$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="V52">
+        <f t="shared" ref="V52:V71" si="33">ROUND((($B53-V$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="W52">
+        <f t="shared" ref="W52:W71" si="34">ROUND((($B53-W$22) + 1) * 2,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53">
+        <f t="shared" ref="B53:B70" si="35">B52-0.05</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54">
+        <f t="shared" si="35"/>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55">
+        <f t="shared" si="35"/>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56">
+        <f t="shared" si="35"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57">
+        <f t="shared" si="35"/>
+        <v>0.69999999999999973</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58">
+        <f t="shared" si="35"/>
+        <v>0.64999999999999969</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59">
+        <f t="shared" si="35"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60">
+        <f t="shared" si="35"/>
+        <v>0.5499999999999996</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61">
+        <f t="shared" si="35"/>
+        <v>0.49999999999999961</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62">
+        <f t="shared" si="35"/>
+        <v>0.44999999999999962</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63">
+        <f t="shared" si="35"/>
+        <v>0.39999999999999963</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T63">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V63">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64">
+        <f t="shared" si="35"/>
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V64">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W64">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65">
+        <f t="shared" si="35"/>
+        <v>0.29999999999999966</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U65">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V65">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="W65">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66">
+        <f t="shared" si="35"/>
+        <v>0.24999999999999967</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="V66">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67">
+        <f t="shared" si="35"/>
+        <v>0.19999999999999968</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="U67">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W67">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68">
+        <f t="shared" si="35"/>
+        <v>0.14999999999999969</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U68">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V68">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W68">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69">
+        <f t="shared" si="35"/>
+        <v>9.9999999999999686E-2</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V69">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W69">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70">
+        <f t="shared" si="35"/>
+        <v>4.9999999999999684E-2</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V70">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W70">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <f>C72+0.05</f>
+        <v>0.05</v>
+      </c>
+      <c r="E72">
+        <f t="shared" ref="E72" si="36">D72+0.05</f>
+        <v>0.1</v>
+      </c>
+      <c r="F72">
+        <f t="shared" ref="F72" si="37">E72+0.05</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="G72">
+        <f t="shared" ref="G72" si="38">F72+0.05</f>
+        <v>0.2</v>
+      </c>
+      <c r="H72">
+        <f t="shared" ref="H72" si="39">G72+0.05</f>
+        <v>0.25</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72" si="40">H72+0.05</f>
+        <v>0.3</v>
+      </c>
+      <c r="J72">
+        <f t="shared" ref="J72" si="41">I72+0.05</f>
+        <v>0.35</v>
+      </c>
+      <c r="K72">
+        <f t="shared" ref="K72" si="42">J72+0.05</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="L72">
+        <f t="shared" ref="L72" si="43">K72+0.05</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="M72">
+        <f t="shared" ref="M72" si="44">L72+0.05</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="N72">
+        <f t="shared" ref="N72" si="45">M72+0.05</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="O72">
+        <f t="shared" ref="O72" si="46">N72+0.05</f>
+        <v>0.6</v>
+      </c>
+      <c r="P72">
+        <f t="shared" ref="P72" si="47">O72+0.05</f>
+        <v>0.65</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" ref="Q72" si="48">P72+0.05</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="R72">
+        <f t="shared" ref="R72" si="49">Q72+0.05</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="S72">
+        <f t="shared" ref="S72" si="50">R72+0.05</f>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="T72">
+        <f t="shared" ref="T72" si="51">S72+0.05</f>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="U72">
+        <f t="shared" ref="U72" si="52">T72+0.05</f>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="V72">
+        <f t="shared" ref="V72" si="53">U72+0.05</f>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="W72">
+        <f t="shared" ref="W72" si="54">V72+0.05</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="2"/>
+      <c r="V73" s="2"/>
+      <c r="W73" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="C73:W73"/>
     <mergeCell ref="A1:A21"/>
     <mergeCell ref="C23:W23"/>
     <mergeCell ref="A26:A46"/>
     <mergeCell ref="C48:W48"/>
+    <mergeCell ref="A51:A71"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:W21">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:W46">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:W71">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51:W51">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4488,7 +6565,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:W46">
+  <conditionalFormatting sqref="C51:W71">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>